<commit_message>
Uprava rodina - vzor.xlsx
</commit_message>
<xml_diff>
--- a/Genealogy/rodina - vzor.xlsx
+++ b/Genealogy/rodina - vzor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\Neo4j\Genealogy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Neo4j\Genealogy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C8A434-7C65-47AD-B66D-BDF20312EA4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275E1689-1630-49F4-8BF6-BF5AC28E3F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29114" yWindow="785" windowWidth="18851" windowHeight="10303" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="14374" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GEN_person" sheetId="1" r:id="rId1"/>
@@ -308,9 +308,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -394,19 +401,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,430 +706,432 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="10"/>
-    <col min="2" max="2" width="13.21875" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="4.21875" customWidth="1"/>
-    <col min="6" max="6" width="5.5546875" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="2"/>
-    <col min="8" max="8" width="5.109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="3.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="3"/>
-    <col min="13" max="14" width="3.44140625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="13" style="3" customWidth="1"/>
-    <col min="16" max="16" width="14.44140625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="50.21875" customWidth="1"/>
-    <col min="18" max="18" width="32.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4" style="16" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="14" style="15" customWidth="1"/>
+    <col min="5" max="5" width="4.21875" style="15" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" style="15" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="17"/>
+    <col min="8" max="8" width="8.21875" style="17" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" style="17" customWidth="1"/>
+    <col min="10" max="10" width="17" style="17" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" style="17" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="8"/>
+    <col min="13" max="13" width="7" style="8" customWidth="1"/>
+    <col min="14" max="14" width="6.88671875" style="8" customWidth="1"/>
+    <col min="15" max="15" width="13" style="8" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" style="8" customWidth="1"/>
+    <col min="17" max="17" width="45.6640625" style="15" customWidth="1"/>
+    <col min="18" max="18" width="32.44140625" style="15" customWidth="1"/>
+    <col min="19" max="16384" width="8.88671875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8" t="s">
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6" t="str">
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12" t="str">
         <f>CONCATENATE(A2,"-",B2," ",C2," ",D2)</f>
         <v>1-Pavel Horanský Horanský</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7">
+      <c r="F3" s="12"/>
+      <c r="G3" s="13">
         <v>1909</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7" t="s">
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="14">
         <v>1989</v>
       </c>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8" t="s">
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="P3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6" t="str">
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12" t="str">
         <f t="shared" ref="R3:R9" si="0">CONCATENATE(A3,"-",B3," ",C3," ",D3)</f>
         <v>2-Štefan Horanský Horanský</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7">
+      <c r="F4" s="12"/>
+      <c r="G4" s="13">
         <v>1905</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7" t="s">
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="14">
         <v>1985</v>
       </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8" t="s">
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="P4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6" t="str">
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12" t="str">
         <f t="shared" si="0"/>
         <v>3-Zuzana Horanská Budzáková</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7">
+      <c r="F5" s="12"/>
+      <c r="G5" s="13">
         <v>1912</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7" t="s">
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="14">
         <v>1987</v>
       </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8" t="s">
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6" t="str">
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12" t="str">
         <f t="shared" si="0"/>
         <v>4-Mária Košťányová Horanská</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7">
+      <c r="F6" s="12"/>
+      <c r="G6" s="13">
         <v>1902</v>
       </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7" t="s">
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="14">
         <v>1964</v>
       </c>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8" t="s">
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="P6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6" t="str">
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12" t="str">
         <f t="shared" si="0"/>
         <v>5-Aranka Košťányová Kosmálová</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7">
+      <c r="F7" s="12"/>
+      <c r="G7" s="13">
         <v>1903</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7" t="s">
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="14">
         <v>1990</v>
       </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8" t="s">
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="P7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6" t="str">
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12" t="str">
         <f t="shared" si="0"/>
         <v>6-Karolína Košťányová Sobotovičová</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7" t="s">
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8" t="s">
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="P8" s="8" t="s">
+      <c r="P8" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6" t="str">
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12" t="str">
         <f t="shared" si="0"/>
         <v>7-Štefan Košťány Košťány</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7" t="s">
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8" t="s">
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="P9" s="8" t="s">
+      <c r="P9" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6" t="str">
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>8-Jozef Košťány Košťány</v>
       </c>
@@ -1124,6 +1139,7 @@
   </sheetData>
   <autoFilter ref="A1:R9" xr:uid="{C259CC51-9C63-4204-A947-621F7CBE5BFF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1343,12 +1359,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="6" customWidth="1"/>
-    <col min="3" max="5" width="9.5546875" style="7" customWidth="1"/>
-    <col min="6" max="9" width="9.5546875" style="8" customWidth="1"/>
-    <col min="10" max="10" width="34.44140625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="4" customWidth="1"/>
+    <col min="3" max="5" width="9.5546875" style="5" customWidth="1"/>
+    <col min="6" max="9" width="9.5546875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="34.44140625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1358,25 +1374,25 @@
       <c r="B1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>76</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -1387,408 +1403,408 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="6" t="str">
+      <c r="B2" s="4" t="str">
         <f>LEFT(A2, FIND("-",A2)-1)</f>
         <v>2</v>
       </c>
-      <c r="C2" s="7">
-        <v>0</v>
-      </c>
-      <c r="D2" s="7">
-        <v>0</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="8">
-        <v>0</v>
-      </c>
-      <c r="H2" s="8">
-        <v>0</v>
-      </c>
-      <c r="I2" s="8">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6" t="s">
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="6" t="str">
+      <c r="K2" s="4" t="str">
         <f>LEFT(J2, FIND("-",J2)-1)</f>
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="6" t="str">
+      <c r="B3" s="4" t="str">
         <f t="shared" ref="B3:B12" si="0">LEFT(A3, FIND("-",A3)-1)</f>
         <v>36</v>
       </c>
-      <c r="C3" s="7">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8" t="s">
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="8">
-        <v>0</v>
-      </c>
-      <c r="H3" s="8">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6" t="s">
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="K3" s="6" t="str">
+      <c r="K3" s="4" t="str">
         <f t="shared" ref="K3:K12" si="1">LEFT(J3, FIND("-",J3)-1)</f>
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="6" t="str">
+      <c r="B4" s="4" t="str">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C4" s="7">
-        <v>0</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="8">
-        <v>0</v>
-      </c>
-      <c r="H4" s="8">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6" t="s">
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="K4" s="6" t="str">
+      <c r="K4" s="4" t="str">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="6" t="str">
+      <c r="B5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C5" s="7">
-        <v>0</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0</v>
-      </c>
-      <c r="E5" s="7">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="8">
-        <v>0</v>
-      </c>
-      <c r="H5" s="8">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6" t="s">
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="K5" s="6" t="str">
+      <c r="K5" s="4" t="str">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="6" t="str">
+      <c r="B6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C6" s="7">
-        <v>0</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="8">
-        <v>0</v>
-      </c>
-      <c r="H6" s="8">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6" t="s">
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K6" s="6" t="str">
+      <c r="K6" s="4" t="str">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="6" t="str">
+      <c r="B7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C7" s="7">
-        <v>0</v>
-      </c>
-      <c r="D7" s="7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="7">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8" t="s">
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G7" s="8">
-        <v>0</v>
-      </c>
-      <c r="H7" s="8">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6" t="s">
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="6" t="str">
+      <c r="K7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="6" t="str">
+      <c r="B8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C8" s="7">
-        <v>0</v>
-      </c>
-      <c r="D8" s="7">
-        <v>0</v>
-      </c>
-      <c r="E8" s="7">
-        <v>0</v>
-      </c>
-      <c r="F8" s="8" t="s">
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="8">
-        <v>0</v>
-      </c>
-      <c r="H8" s="8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8">
-        <v>0</v>
-      </c>
-      <c r="J8" s="6" t="s">
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="K8" s="6" t="str">
+      <c r="K8" s="4" t="str">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="6" t="str">
+      <c r="B9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C9" s="7">
-        <v>0</v>
-      </c>
-      <c r="D9" s="7">
-        <v>0</v>
-      </c>
-      <c r="E9" s="7">
-        <v>0</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G9" s="8">
-        <v>0</v>
-      </c>
-      <c r="H9" s="8">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8">
-        <v>0</v>
-      </c>
-      <c r="J9" s="6" t="s">
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K9" s="6" t="str">
+      <c r="K9" s="4" t="str">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="6" t="str">
+      <c r="B10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C10" s="7">
-        <v>0</v>
-      </c>
-      <c r="D10" s="7">
-        <v>0</v>
-      </c>
-      <c r="E10" s="7">
-        <v>0</v>
-      </c>
-      <c r="F10" s="8" t="s">
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G10" s="8">
-        <v>0</v>
-      </c>
-      <c r="H10" s="8">
-        <v>0</v>
-      </c>
-      <c r="I10" s="8">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6" t="s">
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K10" s="6" t="str">
+      <c r="K10" s="4" t="str">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="6" t="str">
+      <c r="B11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C11" s="7">
-        <v>0</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0</v>
-      </c>
-      <c r="E11" s="7">
-        <v>0</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="8">
-        <v>0</v>
-      </c>
-      <c r="H11" s="8">
-        <v>0</v>
-      </c>
-      <c r="I11" s="8">
-        <v>0</v>
-      </c>
-      <c r="J11" s="6" t="s">
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K11" s="6" t="str">
+      <c r="K11" s="4" t="str">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="6" t="str">
+      <c r="B12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C12" s="7">
-        <v>0</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0</v>
-      </c>
-      <c r="E12" s="7">
-        <v>0</v>
-      </c>
-      <c r="F12" s="8" t="s">
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G12" s="8">
-        <v>0</v>
-      </c>
-      <c r="H12" s="8">
-        <v>0</v>
-      </c>
-      <c r="I12" s="8">
-        <v>0</v>
-      </c>
-      <c r="J12" s="6" t="s">
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="K12" s="6" t="str">
+      <c r="K12" s="4" t="str">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>

</xml_diff>